<commit_message>
added RAS 2D models and comparison scripts
</commit_message>
<xml_diff>
--- a/results_for_all_cases.xlsx
+++ b/results_for_all_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xzl123\Dropbox\student_thesis\Fikri\LWD_flow_resistance\open_data_repositories\LWD_flow_resistance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EDCB2B-02B1-45E2-A390-EC3F0F926E59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8BC265-94DE-4FCF-A5F5-35D6227DFC81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="69">
   <si>
     <t>Sediment</t>
   </si>
@@ -120,15 +120,9 @@
     <t>Fr_downstream</t>
   </si>
   <si>
-    <t>Manning's n</t>
-  </si>
-  <si>
     <t>Results for all cases</t>
   </si>
   <si>
-    <t>Cd</t>
-  </si>
-  <si>
     <t>cm^3</t>
   </si>
   <si>
@@ -190,6 +184,78 @@
   </si>
   <si>
     <t>Simulated flow partition (using calibrated Cd)</t>
+  </si>
+  <si>
+    <t>HEC-RAS 2D</t>
+  </si>
+  <si>
+    <t>b coff. Estimated from Cd</t>
+  </si>
+  <si>
+    <t>Manning's n (w/o turb.)</t>
+  </si>
+  <si>
+    <t>Manning's n (w/ turb.)</t>
+  </si>
+  <si>
+    <t>b coeff. (w/o turb.)</t>
+  </si>
+  <si>
+    <t>b coeff. (w/ turb.)</t>
+  </si>
+  <si>
+    <t>Cd (w/ turb.)</t>
+  </si>
+  <si>
+    <t>Cd (w/o turb.)</t>
+  </si>
+  <si>
+    <t>ManningN_coarse_1</t>
+  </si>
+  <si>
+    <t>ManningN_coarse_2</t>
+  </si>
+  <si>
+    <t>ManningN_coarse_3</t>
+  </si>
+  <si>
+    <t>Cd_coarse_1</t>
+  </si>
+  <si>
+    <t>Cd_coarse_2</t>
+  </si>
+  <si>
+    <t>Cd_coarse_3</t>
+  </si>
+  <si>
+    <t>SRH-2D caps n values to 10</t>
+  </si>
+  <si>
+    <t>(not working even for large Cd)</t>
+  </si>
+  <si>
+    <t>2000 (not working)</t>
+  </si>
+  <si>
+    <t>1000 (not working)</t>
+  </si>
+  <si>
+    <t>b coeff. coarse 1</t>
+  </si>
+  <si>
+    <t>b coeff. coarse 2</t>
+  </si>
+  <si>
+    <t>b coeff. coarse 3</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Simulated flow partition (using calibrated ManningN)</t>
+  </si>
+  <si>
+    <t>Cd estimated from b</t>
   </si>
 </sst>
 </file>
@@ -262,7 +328,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,12 +358,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -352,9 +412,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -368,16 +428,21 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="5"/>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="5" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="6" fillId="6" borderId="1" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="7" fillId="7" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -665,14 +730,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:T44"/>
+  <dimension ref="C3:U68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="W28" sqref="W28"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63:T65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.81640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
@@ -685,7 +751,7 @@
   <sheetData>
     <row r="3" spans="4:20" x14ac:dyDescent="0.35">
       <c r="H3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="4:20" x14ac:dyDescent="0.35">
@@ -705,26 +771,26 @@
       </c>
     </row>
     <row r="10" spans="4:20" x14ac:dyDescent="0.35">
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="14" t="s">
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
     </row>
     <row r="11" spans="4:20" x14ac:dyDescent="0.35">
       <c r="D11" s="2" t="s">
@@ -952,7 +1018,7 @@
     </row>
     <row r="15" spans="4:20" x14ac:dyDescent="0.35">
       <c r="D15" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E15" s="10">
         <f t="shared" ref="E15:L15" si="0">E14/1.5</f>
@@ -1019,7 +1085,7 @@
         <v>0.10100000000000002</v>
       </c>
     </row>
-    <row r="16" spans="4:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="D16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1088,7 +1154,7 @@
         <v>2.4900000000000033E-2</v>
       </c>
     </row>
-    <row r="17" spans="3:20" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:21" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1141,7 +1207,7 @@
         <v>0.12659999999999999</v>
       </c>
     </row>
-    <row r="18" spans="3:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="D18" s="2" t="s">
         <v>12</v>
       </c>
@@ -1210,7 +1276,7 @@
         <v>83.564356435643546</v>
       </c>
     </row>
-    <row r="19" spans="3:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="D19" s="2" t="s">
         <v>5</v>
       </c>
@@ -1263,7 +1329,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="20" spans="3:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
@@ -1316,7 +1382,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="21" spans="3:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="D21" s="2" t="s">
         <v>7</v>
       </c>
@@ -1369,7 +1435,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="22" spans="3:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
@@ -1438,7 +1504,7 @@
         <v>1.9999999999999962E-2</v>
       </c>
     </row>
-    <row r="23" spans="3:20" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:21" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="D23" s="2" t="s">
         <v>19</v>
       </c>
@@ -1507,7 +1573,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="24" spans="3:20" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:21" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="D24" s="2" t="s">
         <v>20</v>
       </c>
@@ -1576,7 +1642,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="25" spans="3:20" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:21" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="D25" s="2" t="s">
         <v>16</v>
       </c>
@@ -1645,7 +1711,7 @@
         <v>0.28055555555555561</v>
       </c>
     </row>
-    <row r="26" spans="3:20" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:21" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="D26" s="2" t="s">
         <v>17</v>
       </c>
@@ -1714,7 +1780,7 @@
         <v>0.29705882352941182</v>
       </c>
     </row>
-    <row r="27" spans="3:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="D27" s="2" t="s">
         <v>21</v>
       </c>
@@ -1783,7 +1849,7 @@
         <v>0.14929082531996343</v>
       </c>
     </row>
-    <row r="28" spans="3:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="D28" s="2" t="s">
         <v>22</v>
       </c>
@@ -1852,9 +1918,9 @@
         <v>0.16265540319118621</v>
       </c>
     </row>
-    <row r="29" spans="3:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="D29" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E29" s="4">
         <v>4.5</v>
@@ -1881,33 +1947,33 @@
         <v>10.5</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q29" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="S29" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T29" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="3:20" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="3:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="D30" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E30" s="4">
         <f>E29*2.54/100</f>
@@ -1942,303 +2008,1201 @@
         <v>0.26669999999999999</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O30" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q30" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R30" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="S30" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T30" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="3:20" x14ac:dyDescent="0.35">
-      <c r="C31" s="15" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C31" s="16" t="s">
+        <v>39</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="E31">
-        <v>2.1</v>
+        <v>2.13</v>
       </c>
       <c r="F31">
-        <v>2.2000000000000002</v>
+        <v>2.16</v>
       </c>
       <c r="G31">
-        <v>2.5</v>
+        <v>2.66</v>
       </c>
       <c r="H31">
-        <v>2.6</v>
+        <v>2.72</v>
       </c>
       <c r="I31">
-        <v>1.3</v>
+        <v>1.26</v>
       </c>
       <c r="J31">
         <v>1.17</v>
       </c>
       <c r="K31">
-        <v>1.27</v>
+        <v>1.26</v>
       </c>
       <c r="L31">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="M31">
-        <v>2.4</v>
+        <v>2.42</v>
       </c>
       <c r="N31">
         <v>2.36</v>
       </c>
       <c r="O31">
+        <v>1.92</v>
+      </c>
+      <c r="P31">
+        <v>1.98</v>
+      </c>
+      <c r="Q31">
+        <v>2.63</v>
+      </c>
+      <c r="R31">
+        <v>2.37</v>
+      </c>
+      <c r="S31">
+        <v>1.78</v>
+      </c>
+      <c r="T31">
+        <v>1.62</v>
+      </c>
+      <c r="U31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C32" s="16"/>
+      <c r="D32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32">
+        <v>2.25</v>
+      </c>
+      <c r="F32">
+        <v>2.36</v>
+      </c>
+      <c r="G32">
+        <v>2.73</v>
+      </c>
+      <c r="H32">
+        <v>2.83</v>
+      </c>
+      <c r="I32">
+        <v>1.3</v>
+      </c>
+      <c r="J32">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="K32">
+        <v>1.24</v>
+      </c>
+      <c r="L32">
+        <v>1.44</v>
+      </c>
+      <c r="M32">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="N32">
+        <v>2.5</v>
+      </c>
+      <c r="O32">
+        <v>1.95</v>
+      </c>
+      <c r="P32">
+        <v>2</v>
+      </c>
+      <c r="Q32">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="R32">
+        <v>2.33</v>
+      </c>
+      <c r="S32">
         <v>1.82</v>
       </c>
-      <c r="P31">
-        <v>1.97</v>
-      </c>
-      <c r="Q31">
-        <v>2.64</v>
-      </c>
-      <c r="R31">
-        <v>2.38</v>
-      </c>
-      <c r="S31">
-        <v>1.8</v>
-      </c>
-      <c r="T31">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="32" spans="3:20" x14ac:dyDescent="0.35">
-      <c r="C32" s="15"/>
-      <c r="D32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="11">
-        <v>36.5</v>
-      </c>
-      <c r="F32" s="11">
-        <v>34.4</v>
-      </c>
-      <c r="G32">
-        <v>58.3</v>
-      </c>
-      <c r="H32">
+      <c r="T32">
+        <v>1.9</v>
+      </c>
+      <c r="U32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C33" s="16"/>
+      <c r="D33" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33">
+        <v>36.4</v>
+      </c>
+      <c r="F33">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="G33">
+        <v>58.6</v>
+      </c>
+      <c r="H33">
         <v>53.4</v>
       </c>
-      <c r="I32">
-        <v>16.5</v>
-      </c>
-      <c r="J32">
-        <v>14.1</v>
-      </c>
-      <c r="K32">
-        <v>20.5</v>
-      </c>
-      <c r="L32">
-        <v>25.6</v>
-      </c>
-      <c r="M32">
-        <v>60</v>
-      </c>
-      <c r="N32">
-        <v>56.1</v>
-      </c>
-      <c r="O32">
-        <v>51.5</v>
-      </c>
-      <c r="P32">
+      <c r="I33">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="J33">
+        <v>14</v>
+      </c>
+      <c r="K33">
+        <v>20.3</v>
+      </c>
+      <c r="L33">
+        <v>25.4</v>
+      </c>
+      <c r="M33">
+        <v>58.9</v>
+      </c>
+      <c r="N33">
+        <v>56</v>
+      </c>
+      <c r="O33">
+        <v>51.2</v>
+      </c>
+      <c r="P33">
+        <v>51.3</v>
+      </c>
+      <c r="Q33">
+        <v>64.2</v>
+      </c>
+      <c r="R33">
+        <v>53.2</v>
+      </c>
+      <c r="S33">
+        <v>43.8</v>
+      </c>
+      <c r="T33">
+        <v>38.1</v>
+      </c>
+      <c r="U33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C34" s="16"/>
+      <c r="D34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34">
+        <v>37.1</v>
+      </c>
+      <c r="F34">
+        <v>35</v>
+      </c>
+      <c r="G34">
+        <v>60.4</v>
+      </c>
+      <c r="H34">
+        <v>55</v>
+      </c>
+      <c r="I34">
+        <v>15.5</v>
+      </c>
+      <c r="J34">
+        <v>11.5</v>
+      </c>
+      <c r="K34">
+        <v>17.5</v>
+      </c>
+      <c r="L34">
+        <v>23</v>
+      </c>
+      <c r="M34">
+        <v>61.1</v>
+      </c>
+      <c r="N34">
+        <v>57.5</v>
+      </c>
+      <c r="O34">
         <v>52.5</v>
       </c>
-      <c r="Q32">
-        <v>64.8</v>
-      </c>
-      <c r="R32">
-        <v>53.4</v>
-      </c>
-      <c r="S32">
-        <v>45.4</v>
-      </c>
-      <c r="T32">
+      <c r="P34">
+        <v>52.5</v>
+      </c>
+      <c r="Q34">
+        <v>55.8</v>
+      </c>
+      <c r="R34">
+        <v>49.1</v>
+      </c>
+      <c r="S34">
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="3:20" x14ac:dyDescent="0.35">
-      <c r="C33" s="15"/>
-    </row>
-    <row r="34" spans="3:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="C34" s="15"/>
-      <c r="D34" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34">
+      <c r="T34">
+        <v>34.9</v>
+      </c>
+    </row>
+    <row r="35" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C35" s="16"/>
+    </row>
+    <row r="36" spans="3:21" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C36" s="16"/>
+      <c r="D36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I36">
+        <f>0.0917419598 /(0.0917419598+0.026327734)</f>
+        <v>0.77701531059615581</v>
+      </c>
+      <c r="J36">
+        <f>0.114413312/(0.114413312+ 0.0332896474)</f>
+        <v>0.77461760051911321</v>
+      </c>
+      <c r="K36">
+        <f>0.0983932587/(0.0983932587+ 0.0209328895)</f>
+        <v>0.82457416236284753</v>
+      </c>
+      <c r="L36">
+        <f>0.119549756 /(0.119549756+ 0.0244502382)</f>
+        <v>0.83020667232776879</v>
+      </c>
+      <c r="Q36">
+        <f>0.104324455/(0.104324455+ 0.0156771081)</f>
+        <v>0.8693591342061443</v>
+      </c>
+      <c r="R36">
+        <f>0.129448942/(0.129448942+ 0.0215516987)</f>
+        <v>0.85727412413555404</v>
+      </c>
+      <c r="S36">
+        <f>0.101843516/(0.101843516+ 0.0181567726)</f>
+        <v>0.84869392555777567</v>
+      </c>
+      <c r="T36">
+        <f>0.127135164/(0.127135164+ 0.0248645603)</f>
+        <v>0.83641706973806662</v>
+      </c>
+    </row>
+    <row r="37" spans="3:21" ht="29" x14ac:dyDescent="0.35">
+      <c r="C37" s="16"/>
+      <c r="D37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37">
         <v>0</v>
       </c>
-      <c r="F34">
+      <c r="F37">
         <v>0</v>
       </c>
-      <c r="G34">
+      <c r="G37">
         <v>0</v>
       </c>
-      <c r="H34">
+      <c r="H37">
         <v>0</v>
       </c>
-      <c r="I34">
+      <c r="I37">
         <v>0.77900000000000003</v>
       </c>
-      <c r="J34">
+      <c r="J37">
         <v>0.77700000000000002</v>
       </c>
-      <c r="K34">
+      <c r="K37">
         <v>0.82299999999999995</v>
       </c>
-      <c r="L34">
+      <c r="L37">
         <v>0.83099999999999996</v>
       </c>
-      <c r="M34">
+      <c r="M37">
         <v>0</v>
       </c>
-      <c r="N34">
+      <c r="N37">
         <v>0</v>
       </c>
-      <c r="O34">
+      <c r="O37">
         <v>0</v>
       </c>
-      <c r="P34">
+      <c r="P37">
         <v>0</v>
       </c>
-      <c r="Q34">
+      <c r="Q37">
         <v>0.86799999999999999</v>
       </c>
-      <c r="R34">
+      <c r="R37">
         <v>0.85599999999999998</v>
       </c>
-      <c r="S34">
+      <c r="S37">
         <v>0.84599999999999997</v>
       </c>
-      <c r="T34">
+      <c r="T37">
         <v>0.83699999999999997</v>
       </c>
     </row>
-    <row r="35" spans="3:20" x14ac:dyDescent="0.35">
-      <c r="C35" s="15"/>
-    </row>
-    <row r="36" spans="3:20" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="C36" s="15"/>
-      <c r="D36" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E36" s="12">
+    <row r="38" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C38" s="16"/>
+    </row>
+    <row r="39" spans="3:21" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C39" s="16"/>
+      <c r="D39" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" s="11">
         <f>2*9.8*0.2*E31^2/((E23+E24)/2)^(4/3)</f>
-        <v>32.350770844181419</v>
-      </c>
-      <c r="F36" s="12">
-        <f t="shared" ref="F36:T36" si="18">2*9.8*0.2*F31^2/((F23+F24)/2)^(4/3)</f>
-        <v>35.505154395881647</v>
-      </c>
-      <c r="G36" s="12">
+        <v>33.281680780718062</v>
+      </c>
+      <c r="F39" s="11">
+        <f t="shared" ref="F39:T39" si="18">2*9.8*0.2*F31^2/((F23+F24)/2)^(4/3)</f>
+        <v>34.225795113517655</v>
+      </c>
+      <c r="G39" s="11">
         <f>2*9.8*0.2*G31^2/((G23+G24)/2)^(4/3)</f>
-        <v>63.681506220493667</v>
-      </c>
-      <c r="H36" s="12">
+        <v>72.093578466195993</v>
+      </c>
+      <c r="H39" s="11">
         <f t="shared" si="18"/>
-        <v>70.411172060852621</v>
-      </c>
-      <c r="I36" s="12">
+        <v>77.060653161984035</v>
+      </c>
+      <c r="I39" s="11">
         <f t="shared" si="18"/>
-        <v>12.530945822065508</v>
-      </c>
-      <c r="J36" s="12">
+        <v>11.771674311900119</v>
+      </c>
+      <c r="J39" s="11">
         <f t="shared" si="18"/>
         <v>10.150066115873059</v>
       </c>
-      <c r="K36" s="12">
+      <c r="K39" s="11">
         <f t="shared" si="18"/>
-        <v>15.931873025183457</v>
-      </c>
-      <c r="L36" s="12">
+        <v>15.681965165094711</v>
+      </c>
+      <c r="L39" s="11">
         <f t="shared" si="18"/>
-        <v>25.28711943981007</v>
-      </c>
-      <c r="M36" s="12">
+        <v>22.225007320145561</v>
+      </c>
+      <c r="M39" s="11">
         <f t="shared" si="18"/>
-        <v>60.078659499654563</v>
-      </c>
-      <c r="N36" s="12">
+        <v>61.084142620447402</v>
+      </c>
+      <c r="N39" s="11">
         <f t="shared" si="18"/>
         <v>58.092726032860426</v>
       </c>
-      <c r="O36" s="12">
+      <c r="O39" s="11">
         <f t="shared" si="18"/>
-        <v>52.642695322679842</v>
-      </c>
-      <c r="P36" s="12">
+        <v>58.586533038741386</v>
+      </c>
+      <c r="P39" s="11">
         <f t="shared" si="18"/>
-        <v>61.677646503377666</v>
-      </c>
-      <c r="Q36" s="12">
+        <v>62.305404764833369</v>
+      </c>
+      <c r="Q39" s="11">
         <f t="shared" si="18"/>
-        <v>72.695177994582039</v>
-      </c>
-      <c r="R36" s="12">
+        <v>72.145499981451508</v>
+      </c>
+      <c r="R39" s="11">
         <f t="shared" si="18"/>
-        <v>59.081520637125571</v>
-      </c>
-      <c r="S36" s="12">
+        <v>58.58608030271003</v>
+      </c>
+      <c r="S39" s="11">
         <f t="shared" si="18"/>
-        <v>51.986590079794674</v>
-      </c>
-      <c r="T36" s="12">
+        <v>50.837750620006616</v>
+      </c>
+      <c r="T39" s="11">
         <f t="shared" si="18"/>
-        <v>45.929655078657383</v>
-      </c>
-    </row>
-    <row r="37" spans="3:20" x14ac:dyDescent="0.35">
-      <c r="C37" s="15"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
-      <c r="O37" s="12"/>
-      <c r="P37" s="12"/>
-      <c r="Q37" s="12"/>
-      <c r="R37" s="12"/>
-      <c r="S37" s="12"/>
-      <c r="T37" s="12"/>
-    </row>
-    <row r="42" spans="3:20" x14ac:dyDescent="0.35">
-      <c r="H42" s="5"/>
-    </row>
-    <row r="43" spans="3:20" x14ac:dyDescent="0.35">
-      <c r="H43" s="5"/>
-    </row>
-    <row r="44" spans="3:20" x14ac:dyDescent="0.35">
-      <c r="H44" s="6"/>
+        <v>41.708576743400855</v>
+      </c>
+    </row>
+    <row r="40" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C40" s="16"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11"/>
+      <c r="S40" s="11"/>
+      <c r="T40" s="11"/>
+    </row>
+    <row r="41" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C41" s="16"/>
+      <c r="D41" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="13">
+        <v>2.64</v>
+      </c>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13">
+        <v>1.62</v>
+      </c>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13">
+        <v>1.99</v>
+      </c>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
+      <c r="T41" s="13">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="42" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C42" s="16"/>
+      <c r="D42" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="13">
+        <v>2.72</v>
+      </c>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13">
+        <v>1.73</v>
+      </c>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
+      <c r="P42" s="13">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
+      <c r="T42" s="13">
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="43" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C43" s="16"/>
+      <c r="D43" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="14">
+        <v>6.35</v>
+      </c>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13">
+        <v>2.94</v>
+      </c>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
+      <c r="T43" s="15">
+        <v>10</v>
+      </c>
+      <c r="U43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C44" s="16"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
+      <c r="T44" s="11"/>
+    </row>
+    <row r="45" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C45" s="16"/>
+      <c r="D45" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11">
+        <v>62.2</v>
+      </c>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11">
+        <v>28.6</v>
+      </c>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11">
+        <v>64.5</v>
+      </c>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+      <c r="T45" s="11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C46" s="16"/>
+      <c r="D46" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11">
+        <v>107</v>
+      </c>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11">
+        <v>49.9</v>
+      </c>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11">
+        <v>149.80000000000001</v>
+      </c>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="11"/>
+      <c r="T46" s="11">
+        <v>88.6</v>
+      </c>
+    </row>
+    <row r="47" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="C47" s="16"/>
+      <c r="D47" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
+      <c r="T47" s="11">
+        <v>2000</v>
+      </c>
+      <c r="U47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C49" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E49">
+        <v>2.25</v>
+      </c>
+      <c r="F49">
+        <v>2.25</v>
+      </c>
+      <c r="G49">
+        <v>2.66</v>
+      </c>
+      <c r="H49">
+        <v>2.72</v>
+      </c>
+      <c r="I49">
+        <v>1.33</v>
+      </c>
+      <c r="J49">
+        <v>1.18</v>
+      </c>
+      <c r="K49">
+        <v>1.29</v>
+      </c>
+      <c r="L49">
+        <v>1.48</v>
+      </c>
+      <c r="M49">
+        <v>2.46</v>
+      </c>
+      <c r="N49">
+        <v>2.42</v>
+      </c>
+      <c r="O49">
+        <v>1.92</v>
+      </c>
+      <c r="P49">
+        <v>1.96</v>
+      </c>
+      <c r="Q49">
+        <v>2.84</v>
+      </c>
+      <c r="R49">
+        <v>2.54</v>
+      </c>
+      <c r="S49">
+        <v>1.92</v>
+      </c>
+      <c r="T49">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="50" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C50" s="16"/>
+      <c r="D50" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E50">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="F50">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="G50">
+        <v>2.66</v>
+      </c>
+      <c r="H50">
+        <v>2.72</v>
+      </c>
+      <c r="I50">
+        <v>1.31</v>
+      </c>
+      <c r="J50">
+        <v>1.18</v>
+      </c>
+      <c r="K50">
+        <v>1.35</v>
+      </c>
+      <c r="L50">
+        <v>1.49</v>
+      </c>
+      <c r="M50">
+        <v>2.56</v>
+      </c>
+      <c r="N50">
+        <v>2.42</v>
+      </c>
+      <c r="O50">
+        <v>1.91</v>
+      </c>
+      <c r="P50">
+        <v>1.93</v>
+      </c>
+      <c r="Q50">
+        <v>2.84</v>
+      </c>
+      <c r="R50">
+        <v>2.34</v>
+      </c>
+      <c r="S50">
+        <v>1.98</v>
+      </c>
+      <c r="T50">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="51" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C51" s="16"/>
+      <c r="D51" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E51">
+        <v>78.2</v>
+      </c>
+      <c r="F51">
+        <v>79.3</v>
+      </c>
+      <c r="G51">
+        <v>122.9</v>
+      </c>
+      <c r="H51">
+        <v>121.1</v>
+      </c>
+      <c r="I51">
+        <v>35.4</v>
+      </c>
+      <c r="J51">
+        <v>34.9</v>
+      </c>
+      <c r="K51">
+        <v>42.5</v>
+      </c>
+      <c r="L51">
+        <v>59.2</v>
+      </c>
+      <c r="M51">
+        <v>146.30000000000001</v>
+      </c>
+      <c r="N51">
+        <v>130.1</v>
+      </c>
+      <c r="O51">
+        <v>115.6</v>
+      </c>
+      <c r="P51">
+        <v>118.1</v>
+      </c>
+      <c r="Q51">
+        <v>149.5</v>
+      </c>
+      <c r="R51">
+        <v>124.6</v>
+      </c>
+      <c r="S51">
+        <v>107.4</v>
+      </c>
+      <c r="T51">
+        <v>94.9</v>
+      </c>
+    </row>
+    <row r="52" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C52" s="16"/>
+      <c r="D52" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E52">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="F52">
+        <v>79.2</v>
+      </c>
+      <c r="G52">
+        <v>122.7</v>
+      </c>
+      <c r="H52">
+        <v>120.9</v>
+      </c>
+      <c r="I52">
+        <v>39</v>
+      </c>
+      <c r="J52">
+        <v>30</v>
+      </c>
+      <c r="K52">
+        <v>46.2</v>
+      </c>
+      <c r="L52">
+        <v>56.7</v>
+      </c>
+      <c r="M52">
+        <v>140</v>
+      </c>
+      <c r="N52">
+        <v>130</v>
+      </c>
+      <c r="O52">
+        <v>115.6</v>
+      </c>
+      <c r="P52">
+        <v>118.2</v>
+      </c>
+      <c r="Q52">
+        <v>149.5</v>
+      </c>
+      <c r="R52">
+        <v>124.6</v>
+      </c>
+      <c r="S52">
+        <v>104</v>
+      </c>
+      <c r="T52">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="53" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C53" s="16"/>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C54" s="16"/>
+      <c r="D54" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E54">
+        <f>E33/2/0.2</f>
+        <v>90.999999999999986</v>
+      </c>
+      <c r="F54">
+        <f t="shared" ref="F54:T54" si="19">F33/2/0.2</f>
+        <v>85.5</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="19"/>
+        <v>146.5</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="19"/>
+        <v>133.5</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="19"/>
+        <v>40.999999999999993</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="19"/>
+        <v>35</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="19"/>
+        <v>50.75</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="19"/>
+        <v>63.499999999999993</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="19"/>
+        <v>147.25</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="19"/>
+        <v>140</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="19"/>
+        <v>128</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="19"/>
+        <v>128.24999999999997</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="19"/>
+        <v>160.5</v>
+      </c>
+      <c r="R54">
+        <f t="shared" si="19"/>
+        <v>133</v>
+      </c>
+      <c r="S54">
+        <f t="shared" si="19"/>
+        <v>109.49999999999999</v>
+      </c>
+      <c r="T54">
+        <f t="shared" si="19"/>
+        <v>95.25</v>
+      </c>
+    </row>
+    <row r="55" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C55" s="12"/>
+      <c r="D55" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E55">
+        <f>E52*2*0.2</f>
+        <v>31.24</v>
+      </c>
+      <c r="F55">
+        <f t="shared" ref="F55:T55" si="20">F52*2*0.2</f>
+        <v>31.680000000000003</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="20"/>
+        <v>49.080000000000005</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="20"/>
+        <v>48.360000000000007</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="20"/>
+        <v>15.600000000000001</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="20"/>
+        <v>12</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="20"/>
+        <v>18.48</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="20"/>
+        <v>22.680000000000003</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="20"/>
+        <v>56</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="20"/>
+        <v>52</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="20"/>
+        <v>46.24</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="20"/>
+        <v>47.28</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="20"/>
+        <v>59.800000000000004</v>
+      </c>
+      <c r="R55">
+        <f t="shared" si="20"/>
+        <v>49.84</v>
+      </c>
+      <c r="S55">
+        <f t="shared" si="20"/>
+        <v>41.6</v>
+      </c>
+      <c r="T55">
+        <f t="shared" si="20"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="3:20" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C56" s="12"/>
+      <c r="D56" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I56">
+        <v>0.77846058018354303</v>
+      </c>
+      <c r="J56">
+        <v>0.77269935110271804</v>
+      </c>
+      <c r="K56">
+        <v>0.82786740742494103</v>
+      </c>
+      <c r="L56">
+        <v>0.82857307710593697</v>
+      </c>
+      <c r="Q56">
+        <v>0.87077396961971598</v>
+      </c>
+      <c r="R56">
+        <v>0.84992591511445903</v>
+      </c>
+      <c r="S56">
+        <v>0.85401873670498896</v>
+      </c>
+      <c r="T56">
+        <v>0.84178600794941205</v>
+      </c>
+    </row>
+    <row r="57" spans="3:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="C57" s="16"/>
+      <c r="D57" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H57" s="6"/>
+      <c r="I57">
+        <v>0.77824210344682099</v>
+      </c>
+      <c r="J57">
+        <v>0.77096971432765904</v>
+      </c>
+      <c r="K57">
+        <v>0.82315928625998802</v>
+      </c>
+      <c r="L57">
+        <v>0.83078528288935105</v>
+      </c>
+      <c r="Q57">
+        <v>0.86711564379642603</v>
+      </c>
+      <c r="R57">
+        <v>0.85764300694281403</v>
+      </c>
+      <c r="S57">
+        <v>0.84590994669981601</v>
+      </c>
+      <c r="T57">
+        <v>0.83268398682031397</v>
+      </c>
+    </row>
+    <row r="58" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C58" s="16"/>
+    </row>
+    <row r="59" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C59" s="16"/>
+      <c r="D59" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H59">
+        <v>2.78</v>
+      </c>
+      <c r="L59">
+        <v>1.5</v>
+      </c>
+      <c r="P59">
+        <v>2.08</v>
+      </c>
+      <c r="T59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C60" s="16"/>
+      <c r="D60" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H60">
+        <v>2.73</v>
+      </c>
+      <c r="L60">
+        <v>1.73</v>
+      </c>
+      <c r="P60">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="T60">
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="61" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C61" s="16"/>
+      <c r="D61" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H61">
+        <v>2.93</v>
+      </c>
+      <c r="L61">
+        <v>6.5</v>
+      </c>
+      <c r="P61">
+        <v>2.6</v>
+      </c>
+      <c r="T61">
+        <v>6.87</v>
+      </c>
+    </row>
+    <row r="62" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C62" s="16"/>
+    </row>
+    <row r="63" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C63" s="16"/>
+      <c r="D63" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H63">
+        <v>113.6</v>
+      </c>
+      <c r="L63">
+        <v>56.7</v>
+      </c>
+      <c r="P63">
+        <v>113.6</v>
+      </c>
+      <c r="T63">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C64" s="16"/>
+      <c r="D64" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H64">
+        <v>190.7</v>
+      </c>
+      <c r="L64">
+        <v>111.2</v>
+      </c>
+      <c r="P64">
+        <v>184</v>
+      </c>
+      <c r="T64">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="65" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C65" s="16"/>
+      <c r="D65" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H65">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="L65">
+        <v>300</v>
+      </c>
+      <c r="P65">
+        <v>82.4</v>
+      </c>
+      <c r="T65">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="66" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C66" s="16"/>
+    </row>
+    <row r="67" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C67" s="16"/>
+    </row>
+    <row r="68" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C68" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="C63:C68"/>
     <mergeCell ref="E10:L10"/>
     <mergeCell ref="M10:T10"/>
-    <mergeCell ref="C31:C37"/>
+    <mergeCell ref="C31:C47"/>
+    <mergeCell ref="C49:C54"/>
+    <mergeCell ref="C57:C62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2246,10 +3210,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2BDFD0D-9602-47A5-B6A3-F95EADBEF8AC}">
-  <dimension ref="G11:I22"/>
+  <dimension ref="G11:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2260,46 +3224,46 @@
   <sheetData>
     <row r="11" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H11">
         <v>0.152</v>
       </c>
       <c r="I11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H12">
         <v>0.2</v>
       </c>
       <c r="I12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H13">
         <v>0.73</v>
       </c>
       <c r="I13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H17">
         <v>74779</v>
       </c>
       <c r="I17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="7:9" x14ac:dyDescent="0.35">
@@ -2308,54 +3272,60 @@
         <v>7.4778999999999998E-2</v>
       </c>
       <c r="I18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H19">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H20">
         <f>H18/(3.14/4*H19^2/H11)</f>
         <v>64.353336164189656</v>
       </c>
       <c r="I20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H21">
         <f>H20/H12/H13</f>
         <v>440.7762750971894</v>
       </c>
       <c r="I21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H22">
         <f>H21*H19</f>
         <v>6.6116441264578407</v>
       </c>
       <c r="I22" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G33">
+        <f>0.2/4</f>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>